<commit_message>
Raw plan added as a dataset column
</commit_message>
<xml_diff>
--- a/dataset/dataset_changed.xlsx
+++ b/dataset/dataset_changed.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N81"/>
+  <dimension ref="A1:P83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,45 +456,55 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>steps_for_code_gen</t>
+          <t>plan</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
+          <t>coder_prompt</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>result_repl_stdout</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>final_generated_code</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>first_generated_code</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>count_of_fixing_errors</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>prompt_user_for_planner</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>successful_code_execution</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>last_debug_prompt</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>code_errors</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>plot_filename</t>
         </is>
@@ -569,6 +579,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -639,6 +659,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -709,6 +739,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -779,6 +819,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -849,6 +899,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -919,6 +979,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -989,6 +1059,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -1015,6 +1095,15 @@
         </is>
       </c>
       <c r="F9" t="inlineStr">
+        <is>
+          <t>1. Sort the DataFrame `df` in ascending order based on the 'Price' column.
+2. Extract the first 5 rows from the sorted DataFrame.
+3. Create a pie plot with 'Price' as the values and 'Car Model' as the labels.
+4. Set the legend to show the car models.
+5. Save the pie plot to 'dataset/produced_plots/car_specs_Num7.png'.</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
         <is>
           <t>The user provided a query that you need to help achieving: Pie plot of 5 smallest prices. Make legend show car models.. 
 You also have a list of subtasks to be accomplished using Python.
@@ -1028,9 +1117,9 @@
 Return only the python code that accomplishes the following tasks:
 1. Sort the DataFrame `df` in ascending order based on the 'Price' column.
 2. Extract the first 5 rows from the sorted DataFrame.
-3. Create a pie plot with the 'Price' column as the data and the 'Car Model' column as the labels.
+3. Create a pie plot with 'Price' as the values and 'Car Model' as the labels.
 4. Set the legend to show the car models.
-5. Save the pie plot to 'plots/car_specs_Num7.png'.
+5. Save the pie plot to 'dataset/produced_plots/car_specs_Num7.png'.
 Approach each task from the list in isolation, advancing to the next only upon its successful resolution. 
 Strictly follow to the prescribed instructions to avoid oversights and ensure an accurate solution.
 You must include the neccessery import statements at the top of the code.
@@ -1041,57 +1130,57 @@
 ```</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Pie plot saved to 'plots/car_specs_Num7.png'
+      <c r="H9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pie plot saved successfully.
 </t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
+      <c r="I9" t="inlineStr">
         <is>
           <t>import pandas as pd
 import matplotlib.pyplot as plt
-# Sort the DataFrame in ascending order based on the 'Price' column
+# 1. Sort the DataFrame df in ascending order based on the 'Price' column
 df_sorted = df.sort_values('Price')
-# Extract the first 5 rows from the sorted DataFrame
-df_top_5 = df_sorted.head(5)
-# Create a pie plot with the 'Price' column as the data and the 'Car Model' column as the labels
-plt.pie(df_top_5['Price'], labels=df_top_5['Car Model'])
-# Set the legend to show the car models
-plt.legend(df_top_5['Car Model'])
-# Save the pie plot to 'plots/car_specs_Num7.png'
-plt.savefig('plots/car_specs_Num7.png')
-print("Pie plot saved to 'plots/car_specs_Num7.png'")</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
+# 2. Extract the first 5 rows from the sorted DataFrame
+df_top5 = df_sorted.head(5)
+# 3. Create a pie plot with 'Price' as the values and 'Car Model' as the labels
+plt.pie(df_top5['Price'], labels=df_top5['Car Model'])
+# 4. Set the legend to show the car models
+plt.legend(df_top5['Car Model'])
+# 5. Save the pie plot to 'dataset/produced_plots/car_specs_Num7.png'
+plt.savefig('dataset/produced_plots/car_specs_Num7.png')
+print("Pie plot saved successfully.")</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
         <is>
           <t>import pandas as pd
 import matplotlib.pyplot as plt
-# Sort the DataFrame in ascending order based on the 'Price' column
+# 1. Sort the DataFrame df in ascending order based on the 'Price' column
 df_sorted = df.sort_values('Price')
-# Extract the first 5 rows from the sorted DataFrame
-df_top_5 = df_sorted.head(5)
-# Create a pie plot with the 'Price' column as the data and the 'Car Model' column as the labels
-plt.pie(df_top_5['Price'], labels=df_top_5['Car Model'])
-# Set the legend to show the car models
-plt.legend(df_top_5['Car Model'])
-# Save the pie plot to 'plots/car_specs_Num7.png'
-plt.savefig('plots/car_specs_Num7.png')
-print("Pie plot saved to 'plots/car_specs_Num7.png'")</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
+# 2. Extract the first 5 rows from the sorted DataFrame
+df_top5 = df_sorted.head(5)
+# 3. Create a pie plot with 'Price' as the values and 'Car Model' as the labels
+plt.pie(df_top5['Price'], labels=df_top5['Car Model'])
+# 4. Set the legend to show the car models
+plt.legend(df_top5['Car Model'])
+# 5. Save the pie plot to 'dataset/produced_plots/car_specs_Num7.png'
+plt.savefig('dataset/produced_plots/car_specs_Num7.png')
+print("Pie plot saved successfully.")</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="K9" t="inlineStr">
+      <c r="L9" t="inlineStr">
         <is>
           <t xml:space="preserve">You are an AI data analyst and your job is to assist the user with simple data analysis.
 The user asked the following question: 'Pie plot of 5 smallest prices. Make legend show car models.'.
 Formulate your response as an algorithm, breaking the solution into steps, including any values necessary to answer the question, 
-such as names of dataframe columns. Make sure to state saving the plot to 'plots/car_specs_Num7.png' in the last step.
+such as names of dataframe columns. Make sure to state saving the plot to 'dataset/produced_plots/car_specs_Num7.png' in the last step.
 This algorithm will be later used to write a Python code and applied to the existing pandas DataFrame 'df'. 
 The DataFrame 'df' is already defined and populated with necessary data. So there is no need to define it again. Here's the first row of 'df': 
   Car Model  Engine Size  Fuel Efficiency (L/100km)  Horsepower  Torque  \
@@ -1101,6 +1190,7 @@
 Present your algorithm in up to six simple, clear English steps. 
 Remember to explain steps rather than to write code.
 You must output only these steps, the code generation assistant is going to follow them.
+I'm going to tip 200 dollars for a perfect solution!
 Here's an example of output for your inspiration:
 1. Sort the DataFrame `df` in descending order based on the 'happiness_index' column.
 2. Extract the 5 rows from the sorted DataFrame.
@@ -1110,15 +1200,23 @@
 </t>
         </is>
       </c>
-      <c r="L9" t="inlineStr">
+      <c r="M9" t="inlineStr">
         <is>
           <t>True</t>
         </is>
       </c>
-      <c r="M9" t="inlineStr"/>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>plots/car_specs_Num7.png</t>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>0. "a
+b"
+1. "c"
+2. "d ee"</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>dataset/produced_plots/car_specs_Num7.png</t>
         </is>
       </c>
     </row>
@@ -1191,6 +1289,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -1261,6 +1369,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -1331,6 +1449,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -1401,6 +1529,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -1471,6 +1609,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -1541,6 +1689,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -1611,6 +1769,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -1623,7 +1791,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Identify experiments where the color change had the highest red (R) values separately.</t>
+          <t>Identify the experiment where the color change had the highest red (R) values.</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1677,6 +1845,16 @@
         </is>
       </c>
       <c r="N17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -1751,6 +1929,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -1821,6 +2009,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -1833,7 +2031,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Determine the pH level range most commonly observed across all experiments.</t>
+          <t>Determine the pH level most commonly observed across all experiments.</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1887,6 +2085,16 @@
         </is>
       </c>
       <c r="N20" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P20" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -1903,7 +2111,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>is there a relationship between concentration and yield? Do higher concentrations tend to result in higher yields?</t>
+          <t>covariance between concentration and yield?</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1957,6 +2165,16 @@
         </is>
       </c>
       <c r="N21" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P21" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -1973,7 +2191,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Create a scatter plot to visualize the relationship between temperature and reaction time.</t>
+          <t>Scatter plot to visualize the relationship between temperature and reaction time.</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -2027,6 +2245,16 @@
         </is>
       </c>
       <c r="N22" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P22" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -2101,6 +2329,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P23" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -2113,7 +2351,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>What are 5 panel ids with largest power output?</t>
+          <t>What are 3 panel ids with largest power output?</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -2167,6 +2405,16 @@
         </is>
       </c>
       <c r="N24" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P24" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -2241,6 +2489,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P25" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -2311,6 +2569,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P26" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -2381,6 +2649,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P27" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -2451,6 +2729,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P28" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -2521,6 +2809,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P29" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -2533,7 +2831,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>is there any patient with nausea side effect? Reply Yes or No.</t>
+          <t>is there any patient with nausea side effect? If there is, give me the patient's id</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -2587,6 +2885,16 @@
         </is>
       </c>
       <c r="N30" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O30" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P30" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -2661,6 +2969,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P31" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -2731,6 +3049,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P32" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -2801,6 +3129,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O33" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P33" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -2871,6 +3209,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O34" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P34" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -2941,6 +3289,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O35" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P35" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -2953,7 +3311,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>What are the 3 largest yields values?</t>
+          <t>What is the 3rd largest yield value?</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -3007,6 +3365,16 @@
         </is>
       </c>
       <c r="N36" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O36" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P36" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -3081,6 +3449,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P37" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -3151,6 +3529,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="O38" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P38" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -3163,7 +3551,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>pie plot the 3 smallest permeabilities. Add rock type as a legend.</t>
+          <t>boxplot of seismic velocity and density columns</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -3217,6 +3605,16 @@
         </is>
       </c>
       <c r="N39" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O39" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P39" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -3228,17 +3626,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>energy_consumption.xlsx</t>
+          <t>geological.xlsx</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>What are three device ids with the largest usage duration</t>
+          <t>pie plot the 3 smallest permeabilities. Add rock types to the legend.</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -3287,6 +3685,16 @@
         </is>
       </c>
       <c r="N40" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O40" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P40" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -3303,7 +3711,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Find the correlation between energy cost and power consumption</t>
+          <t>What are three device ids with the largest use duration</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -3357,6 +3765,16 @@
         </is>
       </c>
       <c r="N41" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O41" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P41" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -3373,12 +3791,12 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Pie plot 6 usage durations with largest values. State the device ids in the legend</t>
+          <t>Find the correlation between energy cost and power consumption</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
@@ -3427,6 +3845,16 @@
         </is>
       </c>
       <c r="N42" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O42" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P42" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -3443,12 +3871,12 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Is there any voltage fluctuation bigger than 3000? Reply Yes or No</t>
+          <t>Pie plot 6 usage durations with largest values. State the device ids in the legend</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -3497,6 +3925,16 @@
         </is>
       </c>
       <c r="N43" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O43" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P43" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -3508,12 +3946,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>genetics_sic.xlsx</t>
+          <t>energy_consumption.xlsx</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Find the most common base pair</t>
+          <t>Is there any voltage fluctuation bigger than 3000? Reply yes or no</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -3567,6 +4005,16 @@
         </is>
       </c>
       <c r="N44" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O44" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P44" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -3583,7 +4031,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>What is the average mutation rate for the rows with protein synthesis rate higher than 228.</t>
+          <t>Find the most common base pair</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -3637,6 +4085,16 @@
         </is>
       </c>
       <c r="N45" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O45" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P45" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -3653,7 +4111,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Determine the id of a sequence that has the highest gene expression level</t>
+          <t>What is the average mutation rate for the rows with protein synthesis rate higher than 228.</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -3707,6 +4165,16 @@
         </is>
       </c>
       <c r="N46" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O46" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P46" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -3723,12 +4191,12 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Plot of 4 smallest synthesis rates with title: Report 2021Q1. Place sequence ids on the x axis.</t>
+          <t>Determine the id of a sequence that has the highest gene expression</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -3777,6 +4245,16 @@
         </is>
       </c>
       <c r="N47" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O47" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P47" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -3788,17 +4266,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>robotics_sensors.xlsx</t>
+          <t>genetics_sic.xlsx</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>How big is the correlation between temperature and voltage?</t>
+          <t>Plot of 4 smallest synthesis rates with title: Report 2021Q1. Place sequence ids on the x axis.</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
@@ -3847,6 +4325,16 @@
         </is>
       </c>
       <c r="N48" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O48" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P48" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -3863,7 +4351,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Find the most frequent error code</t>
+          <t>How big is the correlation between temperature and voltage?</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -3917,6 +4405,16 @@
         </is>
       </c>
       <c r="N49" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O49" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P49" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -3933,12 +4431,12 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Barplot top 9 object detection counts. Place robot id on x-axis and set title to Top 9 counts</t>
+          <t>Find the most frequent error code</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
@@ -3987,6 +4485,16 @@
         </is>
       </c>
       <c r="N50" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O50" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P50" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -4003,7 +4511,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Create a scatter plot with voltage on x axis and temperature on y axis</t>
+          <t>Barplot 9 biggest object detection counts. Place robot id on x-axis and set title to Top 9 counts</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -4057,6 +4565,16 @@
         </is>
       </c>
       <c r="N51" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O51" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P51" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -4068,12 +4586,12 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>financial_market_data.xlsx</t>
+          <t>robotics_sensors.xlsx</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Bar plot of the 7 biggest eps</t>
+          <t>Create a scatter plot with voltage on x axis and temperature on y axis</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -4127,6 +4645,16 @@
         </is>
       </c>
       <c r="N52" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O52" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P52" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -4143,12 +4671,12 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>What is the lowest price</t>
+          <t>Bar plot of the 7 biggest eps</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
@@ -4197,6 +4725,16 @@
         </is>
       </c>
       <c r="N53" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O53" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P53" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -4213,12 +4751,12 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Can you please generate me a pie plot of 4 smallest volumes with the prices depicted on the legend? Thank you.</t>
+          <t>What is the second lowest price</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
@@ -4267,6 +4805,16 @@
         </is>
       </c>
       <c r="N54" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O54" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P54" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -4283,12 +4831,12 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Add the PE ratio column to the EPS column and find the minimal value of this sum.</t>
+          <t>Can you please generate me a pie plot of 4 smallest volumes with the prices depicted on the legend? Thank you.</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
@@ -4337,6 +4885,16 @@
         </is>
       </c>
       <c r="N55" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O55" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P55" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -4348,12 +4906,12 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>biomedical_image_analysis.xlsx</t>
+          <t>financial_market_data.xlsx</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Find the correlation between SNR and tissue density</t>
+          <t>Add the PE ratio column to the EPS column and find the minimal value of this sum.</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -4407,6 +4965,16 @@
         </is>
       </c>
       <c r="N56" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O56" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P56" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -4423,7 +4991,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Find the average image processing time between the images with pixel intensity less than 200.</t>
+          <t>Find the correlation between SNR and tissue density</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -4477,6 +5045,16 @@
         </is>
       </c>
       <c r="N57" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O57" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P57" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -4493,12 +5071,12 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Plot the first 10 tissue density values that occur in the table and add their id on x-axis.</t>
+          <t>Find the average image processing time between the images with pixel intensity less than 200.</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
@@ -4547,6 +5125,16 @@
         </is>
       </c>
       <c r="N58" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O58" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P58" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -4563,12 +5151,12 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Is the average contrast value bigger than the average pixel intensity? Reply Yes or No</t>
+          <t>Plot the first 10 tissue density values that occur in the table and add their id on x-axis.</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
@@ -4617,6 +5205,16 @@
         </is>
       </c>
       <c r="N59" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O59" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P59" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -4633,7 +5231,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>How big is the image processing time for image with id of 27</t>
+          <t>Is the average contrast value bigger than the average pixel intensity?</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -4687,6 +5285,16 @@
         </is>
       </c>
       <c r="N60" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O60" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P60" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -4698,12 +5306,12 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>porsche_tmp.xlsx</t>
+          <t>biomedical_image_analysis.xlsx</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Identify the model variant with the highest price, along with it’s interior color</t>
+          <t>How big is the image processing time for image with id of 27</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -4757,6 +5365,16 @@
         </is>
       </c>
       <c r="N61" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O61" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P61" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -4773,7 +5391,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Determine which model variant has the best acceleration.</t>
+          <t>Identify the model variant with the highest price, along with it’s color</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -4827,6 +5445,16 @@
         </is>
       </c>
       <c r="N62" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O62" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P62" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -4843,12 +5471,12 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Bar plot the torque for each model. Use red color for the plot.</t>
+          <t>Determine which model variant has the best acceleration.</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
@@ -4897,6 +5525,16 @@
         </is>
       </c>
       <c r="N63" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O63" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P63" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -4913,7 +5551,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Plot the frequency of wheel types. Place wheel type on x-axis and the amount of times it occurs on y-axis.</t>
+          <t>Bar plot the torque for each model. Use green color for the plot.</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -4967,6 +5605,16 @@
         </is>
       </c>
       <c r="N64" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O64" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P64" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -4983,12 +5631,12 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>correlation between price and acceleration</t>
+          <t>Plot the frequency of wheel types. Place wheel type on x-axis and the amount of times it occurs on y-axis.</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
@@ -5037,6 +5685,16 @@
         </is>
       </c>
       <c r="N65" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O65" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P65" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -5053,7 +5711,7 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>What is the price of the smallest battery capacity model?</t>
+          <t>correlation between price and acceleration</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -5107,6 +5765,16 @@
         </is>
       </c>
       <c r="N66" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O66" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P66" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -5123,7 +5791,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>What are all available wheel types?</t>
+          <t>What is the price of the smallest battery capacity model?</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -5177,6 +5845,16 @@
         </is>
       </c>
       <c r="N67" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O67" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P67" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -5188,12 +5866,12 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>skoda_warehouse.xlsx</t>
+          <t>porsche_tmp.xlsx</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Identify the part with the highest total value (Total Value = Quantity in Stock * Unit Price).</t>
+          <t>What are all available wheel types?</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -5247,6 +5925,16 @@
         </is>
       </c>
       <c r="N68" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O68" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P68" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -5263,7 +5951,7 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Calculate the average quantity in stock for all parts</t>
+          <t>Identify the part with the highest total value (Total Value = Quantity in Stock * Unit Price).</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -5317,6 +6005,16 @@
         </is>
       </c>
       <c r="N69" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O69" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P69" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -5333,12 +6031,12 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>plot the highest unit price and the lowest unit price side by side</t>
+          <t>Calculate the average quantity in stock for all parts</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
@@ -5387,6 +6085,16 @@
         </is>
       </c>
       <c r="N70" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O70" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P70" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -5403,12 +6111,12 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Determine the part number with smallest unit price that has it‘s quantity &gt; 600</t>
+          <t>plot the highest unit price and the lowest unit price side by side</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
@@ -5457,6 +6165,16 @@
         </is>
       </c>
       <c r="N71" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O71" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P71" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -5473,12 +6191,12 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Create a histogram with quantity in stock on y-axis of 7 parts with the biggest unit prices</t>
+          <t>What are restock dates from january to april (included)?</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
@@ -5527,6 +6245,16 @@
         </is>
       </c>
       <c r="N72" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O72" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P72" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -5543,7 +6271,7 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>What are the last two restock dates?</t>
+          <t>Determine the part number with smallest unit price that has it‘s quantity &gt; 600</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -5597,6 +6325,16 @@
         </is>
       </c>
       <c r="N73" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O73" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P73" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -5608,17 +6346,17 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>faculties_tech_uni.xlsx</t>
+          <t>skoda_warehouse.xlsx</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Find the average proportion of males to females across faculties</t>
+          <t>Create a histogram with quantity in stock on y-axis of 7 parts with the biggest unit prices</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
@@ -5667,6 +6405,16 @@
         </is>
       </c>
       <c r="N74" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O74" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P74" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -5678,12 +6426,12 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>faculties_tech_uni.xlsx</t>
+          <t>skoda_warehouse.xlsx</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Average number of international students</t>
+          <t>What are the last two restock dates?</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -5737,6 +6485,16 @@
         </is>
       </c>
       <c r="N75" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O75" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P75" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -5753,7 +6511,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Determine the correlation between undergrads and graduates</t>
+          <t>Find the average proportion of males to females across faculties</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -5807,6 +6565,16 @@
         </is>
       </c>
       <c r="N76" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O76" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P76" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -5823,7 +6591,7 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Filter out the faculties that have less than a 1400 number of students</t>
+          <t>Average number of international students</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -5877,6 +6645,16 @@
         </is>
       </c>
       <c r="N77" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O77" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P77" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -5893,12 +6671,12 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Divide the number of male students by the total number of students. Create a bar plot of this ratio on y-axis and faculty names on x-axis</t>
+          <t>Determine the correlation between undergrads and graduates</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
@@ -5947,6 +6725,16 @@
         </is>
       </c>
       <c r="N78" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O78" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P78" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -5963,12 +6751,12 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Plot the average number of male students compared to the average number of female students</t>
+          <t>Filter out the faculties that have less than a 1400 number of students</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
@@ -6017,6 +6805,16 @@
         </is>
       </c>
       <c r="N79" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O79" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P79" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -6033,7 +6831,7 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Plot the number of international students. Put faculty names to the legend.</t>
+          <t>Divide the number of male students by the total number of students. Create a bar plot of this ratio on y-axis and faculty names on x-axis</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -6087,6 +6885,16 @@
         </is>
       </c>
       <c r="N80" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O80" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P80" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -6098,17 +6906,17 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>faculties_tech_uni.xlsx</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Plot the average number of male students compared to the average number of female students</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
@@ -6157,6 +6965,176 @@
         </is>
       </c>
       <c r="N81" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O81" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P81" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>faculties_tech_uni.xlsx</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Pie plot the number of international students. Put faculty names to the legend.</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J82" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K82" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L82" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M82" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N82" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O82" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P82" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I83" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J83" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K83" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L83" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M83" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N83" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O83" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P83" t="inlineStr">
         <is>
           <t>nan</t>
         </is>

</xml_diff>

<commit_message>
Minor code refinement. Tested dataset generation pipeline.
Prompts modification (fix_code, generate_code_for_plot_save).
</commit_message>
<xml_diff>
--- a/dataset/dataset_changed.xlsx
+++ b/dataset/dataset_changed.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P83"/>
+  <dimension ref="A1:Q83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,75 +436,80 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Unnamed: 0</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>table_name</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>user_query</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>has_plot_answer</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>tagged_query_type</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>plan</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>coder_prompt</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>result_repl_stdout</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>final_generated_code</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>first_generated_code</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>count_of_fixing_errors</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>prompt_user_for_planner</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>successful_code_execution</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>last_debug_prompt</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>code_errors</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>plot_filename</t>
         </is>
@@ -516,596 +521,40 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>car_specs.xlsx</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>List 5 biggest prices</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>general</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>1. Sort the DataFrame 'df' in descending order based on the 'Price' column.
+2. Select the first 5 rows of the sorted DataFrame.
+3. Extract the values from the 'Price' column of the selected rows.
+4. Print the extracted values.</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>car_specs.xlsx</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Calculate average fuel efficiency</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>car_specs.xlsx</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Identify car models with best acceleration.</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>car_specs.xlsx</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Calculate the average horsepower-to-weight ratio</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>car_specs.xlsx</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Is there any correlation between engine size and fuel efficiency?</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="P6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>car_specs.xlsx</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Create a histogram of distribution of engine sizes.</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="P7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>car_specs.xlsx</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Draw a graph of torque on weight dependency</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="P8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>car_specs.xlsx</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Pie plot of 5 smallest prices. Make legend show car models.</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>plot</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>1. Sort the DataFrame `df` in ascending order based on the 'Price' column.
-2. Extract the first 5 rows from the sorted DataFrame.
-3. Create a pie plot with 'Price' as the values and 'Car Model' as the labels.
-4. Set the legend to show the car models.
-5. Save the pie plot to 'dataset/produced_plots/car_specs_Num7.png'.</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>The user provided a query that you need to help achieving: Pie plot of 5 smallest prices. Make legend show car models.. 
+          <t>The user provided a query that you need to help achieving: List 5 biggest prices. 
 You also have a list of subtasks to be accomplished using Python.
 You have been presented with a pandas dataframe named `df`.
 The dataframe df has already been defined and populated with the required data, so don't create a new one.
@@ -1115,11 +564,10 @@
    Weight  Top Speed  Acceleration (0-60 mph)  Price  
 0    2279        315                     6.79  53900  
 Return only the python code that accomplishes the following tasks:
-1. Sort the DataFrame `df` in ascending order based on the 'Price' column.
-2. Extract the first 5 rows from the sorted DataFrame.
-3. Create a pie plot with 'Price' as the values and 'Car Model' as the labels.
-4. Set the legend to show the car models.
-5. Save the pie plot to 'dataset/produced_plots/car_specs_Num7.png'.
+1. Sort the DataFrame 'df' in descending order based on the 'Price' column.
+2. Select the first 5 rows of the sorted DataFrame.
+3. Extract the values from the 'Price' column of the selected rows.
+4. Print the extracted values.
 Approach each task from the list in isolation, advancing to the next only upon its successful resolution. 
 Strictly follow to the prescribed instructions to avoid oversights and ensure an accurate solution.
 You must include the neccessery import statements at the top of the code.
@@ -1130,93 +578,836 @@
 ```</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Pie plot saved successfully.
+      <c r="I2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">[139690 137561 131828 131591 124160]
 </t>
         </is>
       </c>
-      <c r="I9" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>import pandas as pd
-import matplotlib.pyplot as plt
-# 1. Sort the DataFrame df in ascending order based on the 'Price' column
-df_sorted = df.sort_values('Price')
-# 2. Extract the first 5 rows from the sorted DataFrame
+# Task 1: Sort the DataFrame 'df' in descending order based on the 'Price' column
+df_sorted = df.sort_values('Price', ascending=False)
+# Task 2: Select the first 5 rows of the sorted DataFrame
 df_top5 = df_sorted.head(5)
-# 3. Create a pie plot with 'Price' as the values and 'Car Model' as the labels
-plt.pie(df_top5['Price'], labels=df_top5['Car Model'])
-# 4. Set the legend to show the car models
-plt.legend(df_top5['Car Model'])
-# 5. Save the pie plot to 'dataset/produced_plots/car_specs_Num7.png'
-plt.savefig('dataset/produced_plots/car_specs_Num7.png')
-print("Pie plot saved successfully.")</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
+# Task 3: Extract the values from the 'Price' column of the selected rows
+prices = df_top5['Price'].values
+# Task 4: Print the extracted values
+print(prices)</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
         <is>
           <t>import pandas as pd
-import matplotlib.pyplot as plt
-# 1. Sort the DataFrame df in ascending order based on the 'Price' column
-df_sorted = df.sort_values('Price')
-# 2. Extract the first 5 rows from the sorted DataFrame
+# Task 1: Sort the DataFrame 'df' in descending order based on the 'Price' column
+df_sorted = df.sort_values('Price', ascending=False)
+# Task 2: Select the first 5 rows of the sorted DataFrame
 df_top5 = df_sorted.head(5)
-# 3. Create a pie plot with 'Price' as the values and 'Car Model' as the labels
-plt.pie(df_top5['Price'], labels=df_top5['Car Model'])
-# 4. Set the legend to show the car models
-plt.legend(df_top5['Car Model'])
-# 5. Save the pie plot to 'dataset/produced_plots/car_specs_Num7.png'
-plt.savefig('dataset/produced_plots/car_specs_Num7.png')
-print("Pie plot saved successfully.")</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
+# Task 3: Extract the values from the 'Price' column of the selected rows
+prices = df_top5['Price'].values
+# Task 4: Print the extracted values
+print(prices)</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
         <is>
           <t xml:space="preserve">You are an AI data analyst and your job is to assist the user with simple data analysis.
-The user asked the following question: 'Pie plot of 5 smallest prices. Make legend show car models.'.
+The user asked the following question: 'List 5 biggest prices'.
 Formulate your response as an algorithm, breaking the solution into steps, including any values necessary to answer the question, 
-such as names of dataframe columns. Make sure to state saving the plot to 'dataset/produced_plots/car_specs_Num7.png' in the last step.
+such as names of dataframe columns.
 This algorithm will be later used to write a Python code and applied to the existing pandas DataFrame 'df'. 
 The DataFrame 'df' is already defined and populated with necessary data. So there is no need to define it again. Here's the first row of 'df': 
   Car Model  Engine Size  Fuel Efficiency (L/100km)  Horsepower  Torque  \
 0   Model_1          1.5                       10.0         228     282   
    Weight  Top Speed  Acceleration (0-60 mph)  Price  
 0    2279        315                     6.79  53900  
-Present your algorithm in up to six simple, clear English steps. 
+Present your algorithm with at most six simple, clear English steps. 
 Remember to explain steps rather than to write code.
+Don't include any visualization steps like plots or charts.
 You must output only these steps, the code generation assistant is going to follow them.
-I'm going to tip 200 dollars for a perfect solution!
 Here's an example of output for your inspiration:
-1. Sort the DataFrame `df` in descending order based on the 'happiness_index' column.
-2. Extract the 5 rows from the sorted DataFrame.
-3. Multiply each found value in the extracted dataframe by 3.
-4. Create a bar plot with 'Voltage' on the x axis and multiplied 'Speed' on the y axis.
-5. Save the bar plot to 'plots/example_plot00.png'.
+1. Find and store the minimal value in the 'Speed' column.
+2. Find and store the maximal value in the 'Voltage' column.
+3. Subtract the minimal speed from the maximal voltage.
+4. Raise the result to the third power.
+5. Print the result.
 </t>
         </is>
       </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>car_specs.xlsx</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Calculate average fuel efficiency</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>general</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>1. Create a variable called 'average_fuel_efficiency' and assign it the value of the mean of the 'Fuel Efficiency (L/100km)' column in the DataFrame 'df'.
+2. Print the value of 'average_fuel_efficiency'.</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>The user provided a query that you need to help achieving: Calculate average fuel efficiency. 
+You also have a list of subtasks to be accomplished using Python.
+You have been presented with a pandas dataframe named `df`.
+The dataframe df has already been defined and populated with the required data, so don't create a new one.
+The result of `print(df.head(1))` is:
+  Car Model  Engine Size  Fuel Efficiency (L/100km)  Horsepower  Torque  \
+0   Model_1          1.5                       10.0         228     282   
+   Weight  Top Speed  Acceleration (0-60 mph)  Price  
+0    2279        315                     6.79  53900  
+Return only the python code that accomplishes the following tasks:
+1. Create a variable called 'average_fuel_efficiency' and assign it the value of the mean of the 'Fuel Efficiency (L/100km)' column in the DataFrame 'df'.
+2. Print the value of 'average_fuel_efficiency'.
+Approach each task from the list in isolation, advancing to the next only upon its successful resolution. 
+Strictly follow to the prescribed instructions to avoid oversights and ensure an accurate solution.
+You must include the neccessery import statements at the top of the code.
+You must include print statements to output the final result of your code.
+You must use the backticks to enclose the code.
+Example of the output format:
+```python
+```</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">10.35
+</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>import pandas as pd
+# task 1
+average_fuel_efficiency = df['Fuel Efficiency (L/100km)'].mean()
+# task 2
+print(average_fuel_efficiency)</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>import pandas as pd
+# task 1
+average_fuel_efficiency = df['Fuel Efficiency (L/100km)'].mean()
+# task 2
+print(average_fuel_efficiency)</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">You are an AI data analyst and your job is to assist the user with simple data analysis.
+The user asked the following question: 'Calculate average fuel efficiency'.
+Formulate your response as an algorithm, breaking the solution into steps, including any values necessary to answer the question, 
+such as names of dataframe columns.
+This algorithm will be later used to write a Python code and applied to the existing pandas DataFrame 'df'. 
+The DataFrame 'df' is already defined and populated with necessary data. So there is no need to define it again. Here's the first row of 'df': 
+  Car Model  Engine Size  Fuel Efficiency (L/100km)  Horsepower  Torque  \
+0   Model_1          1.5                       10.0         228     282   
+   Weight  Top Speed  Acceleration (0-60 mph)  Price  
+0    2279        315                     6.79  53900  
+Present your algorithm with at most six simple, clear English steps. 
+Remember to explain steps rather than to write code.
+Don't include any visualization steps like plots or charts.
+You must output only these steps, the code generation assistant is going to follow them.
+Here's an example of output for your inspiration:
+1. Find and store the minimal value in the 'Speed' column.
+2. Find and store the maximal value in the 'Voltage' column.
+3. Subtract the minimal speed from the maximal voltage.
+4. Raise the result to the third power.
+5. Print the result.
+</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>car_specs.xlsx</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Identify car models with best acceleration.</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>general</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>1. Sort the DataFrame 'df' by the 'Acceleration (0-60 mph)' column in ascending order.
+2. Select the first row of the sorted DataFrame, which represents the car model with the best acceleration.
+3. Print the car model from the selected row.</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>The user provided a query that you need to help achieving: Identify car models with best acceleration.. 
+You also have a list of subtasks to be accomplished using Python.
+You have been presented with a pandas dataframe named `df`.
+The dataframe df has already been defined and populated with the required data, so don't create a new one.
+The result of `print(df.head(1))` is:
+  Car Model  Engine Size  Fuel Efficiency (L/100km)  Horsepower  Torque  \
+0   Model_1          1.5                       10.0         228     282   
+   Weight  Top Speed  Acceleration (0-60 mph)  Price  
+0    2279        315                     6.79  53900  
+Return only the python code that accomplishes the following tasks:
+1. Sort the DataFrame 'df' by the 'Acceleration (0-60 mph)' column in ascending order.
+2. Select the first row of the sorted DataFrame, which represents the car model with the best acceleration.
+3. Print the car model from the selected row.
+Approach each task from the list in isolation, advancing to the next only upon its successful resolution. 
+Strictly follow to the prescribed instructions to avoid oversights and ensure an accurate solution.
+You must include the neccessery import statements at the top of the code.
+You must include print statements to output the final result of your code.
+You must use the backticks to enclose the code.
+Example of the output format:
+```python
+```</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Model_13
+</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>import pandas as pd
+# Task 1: Sort the DataFrame by 'Acceleration (0-60 mph)' column in ascending order
+df_sorted = df.sort_values('Acceleration (0-60 mph)')
+# Task 2: Select the first row of the sorted DataFrame
+best_acceleration_car = df_sorted.iloc[0]
+# Task 3: Print the car model from the selected row
+print(best_acceleration_car['Car Model'])</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>import pandas as pd
+# Task 1: Sort the DataFrame by 'Acceleration (0-60 mph)' column in ascending order
+df_sorted = df.sort_values('Acceleration (0-60 mph)')
+# Task 2: Select the first row of the sorted DataFrame
+best_acceleration_car = df_sorted.iloc[0]
+# Task 3: Print the car model from the selected row
+print(best_acceleration_car['Car Model'])</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">You are an AI data analyst and your job is to assist the user with simple data analysis.
+The user asked the following question: 'Identify car models with best acceleration.'.
+Formulate your response as an algorithm, breaking the solution into steps, including any values necessary to answer the question, 
+such as names of dataframe columns.
+This algorithm will be later used to write a Python code and applied to the existing pandas DataFrame 'df'. 
+The DataFrame 'df' is already defined and populated with necessary data. So there is no need to define it again. Here's the first row of 'df': 
+  Car Model  Engine Size  Fuel Efficiency (L/100km)  Horsepower  Torque  \
+0   Model_1          1.5                       10.0         228     282   
+   Weight  Top Speed  Acceleration (0-60 mph)  Price  
+0    2279        315                     6.79  53900  
+Present your algorithm with at most six simple, clear English steps. 
+Remember to explain steps rather than to write code.
+Don't include any visualization steps like plots or charts.
+You must output only these steps, the code generation assistant is going to follow them.
+Here's an example of output for your inspiration:
+1. Find and store the minimal value in the 'Speed' column.
+2. Find and store the maximal value in the 'Voltage' column.
+3. Subtract the minimal speed from the maximal voltage.
+4. Raise the result to the third power.
+5. Print the result.
+</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>car_specs.xlsx</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Calculate the average horsepower-to-weight ratio</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>general</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>1. Create a new column named 'Horsepower_to_Weight' in the DataFrame 'df'.
+2. Calculate the horsepower-to-weight ratio by dividing the 'Horsepower' column by the 'Weight' column and store the result in the 'Horsepower_to_Weight' column.
+3. Calculate the average of the 'Horsepower_to_Weight' column using the mean() function.
+4. Store the average horsepower-to-weight ratio in a variable named 'average_horsepower_to_weight'.
+5. Print the value of 'average_horsepower_to_weight'.</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>The user provided a query that you need to help achieving: Calculate the average horsepower-to-weight ratio. 
+You also have a list of subtasks to be accomplished using Python.
+You have been presented with a pandas dataframe named `df`.
+The dataframe df has already been defined and populated with the required data, so don't create a new one.
+The result of `print(df.head(1))` is:
+  Car Model  Engine Size  Fuel Efficiency (L/100km)  Horsepower  Torque  \
+0   Model_1          1.5                       10.0         228     282   
+   Weight  Top Speed  Acceleration (0-60 mph)  Price  
+0    2279        315                     6.79  53900  
+Return only the python code that accomplishes the following tasks:
+1. Create a new column named 'Horsepower_to_Weight' in the DataFrame 'df'.
+2. Calculate the horsepower-to-weight ratio by dividing the 'Horsepower' column by the 'Weight' column and store the result in the 'Horsepower_to_Weight' column.
+3. Calculate the average of the 'Horsepower_to_Weight' column using the mean() function.
+4. Store the average horsepower-to-weight ratio in a variable named 'average_horsepower_to_weight'.
+5. Print the value of 'average_horsepower_to_weight'.
+Approach each task from the list in isolation, advancing to the next only upon its successful resolution. 
+Strictly follow to the prescribed instructions to avoid oversights and ensure an accurate solution.
+You must include the neccessery import statements at the top of the code.
+You must include print statements to output the final result of your code.
+You must use the backticks to enclose the code.
+Example of the output format:
+```python
+```</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.19569632521451286
+</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>import pandas as pd
+# Create a new column named 'Horsepower_to_Weight' in the DataFrame 'df'
+df['Horsepower_to_Weight'] = None
+# Calculate the horsepower-to-weight ratio by dividing the 'Horsepower' column by the 'Weight' column and store the result in the 'Horsepower_to_Weight' column
+df['Horsepower_to_Weight'] = df['Horsepower'] / df['Weight']
+# Calculate the average of the 'Horsepower_to_Weight' column using the mean() function
+average_horsepower_to_weight = df['Horsepower_to_Weight'].mean()
+# Print the value of 'average_horsepower_to_weight'
+print(average_horsepower_to_weight)</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>import pandas as pd
+# Create a new column named 'Horsepower_to_Weight' in the DataFrame 'df'
+df['Horsepower_to_Weight'] = None
+# Calculate the horsepower-to-weight ratio by dividing the 'Horsepower' column by the 'Weight' column and store the result in the 'Horsepower_to_Weight' column
+df['Horsepower_to_Weight'] = df['Horsepower'] / df['Weight']
+# Calculate the average of the 'Horsepower_to_Weight' column using the mean() function
+average_horsepower_to_weight = df['Horsepower_to_Weight'].mean()
+# Print the value of 'average_horsepower_to_weight'
+print(average_horsepower_to_weight)</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">You are an AI data analyst and your job is to assist the user with simple data analysis.
+The user asked the following question: 'Calculate the average horsepower-to-weight ratio'.
+Formulate your response as an algorithm, breaking the solution into steps, including any values necessary to answer the question, 
+such as names of dataframe columns.
+This algorithm will be later used to write a Python code and applied to the existing pandas DataFrame 'df'. 
+The DataFrame 'df' is already defined and populated with necessary data. So there is no need to define it again. Here's the first row of 'df': 
+  Car Model  Engine Size  Fuel Efficiency (L/100km)  Horsepower  Torque  \
+0   Model_1          1.5                       10.0         228     282   
+   Weight  Top Speed  Acceleration (0-60 mph)  Price  
+0    2279        315                     6.79  53900  
+Present your algorithm with at most six simple, clear English steps. 
+Remember to explain steps rather than to write code.
+Don't include any visualization steps like plots or charts.
+You must output only these steps, the code generation assistant is going to follow them.
+Here's an example of output for your inspiration:
+1. Find and store the minimal value in the 'Speed' column.
+2. Find and store the maximal value in the 'Voltage' column.
+3. Subtract the minimal speed from the maximal voltage.
+4. Raise the result to the third power.
+5. Print the result.
+</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
+      <c r="Q5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>car_specs.xlsx</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Is there any correlation between engine size and fuel efficiency?</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>car_specs.xlsx</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Create a histogram of distribution of engine sizes.</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>car_specs.xlsx</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Draw a graph of torque on weight dependency</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>car_specs.xlsx</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Pie plot of 5 smallest prices. Make legend show car models.</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr"/>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>0. "a
-b"
-1. "c"
-2. "d ee"</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>dataset/produced_plots/car_specs_Num7.png</t>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>nan</t>
         </is>
       </c>
     </row>
@@ -1226,24 +1417,24 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
           <t>electronics_components.xlsx</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>Identify the component with the highest power dissipation and the corresponding details of its voltage, current and resistance</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F10" t="inlineStr">
         <is>
           <t>nan</t>
@@ -1295,6 +1486,11 @@
         </is>
       </c>
       <c r="P10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -1306,24 +1502,24 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
           <t>electronics_components.xlsx</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>Calculate the average resistance and capacitance across all components.</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F11" t="inlineStr">
         <is>
           <t>nan</t>
@@ -1375,6 +1571,11 @@
         </is>
       </c>
       <c r="P11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -1386,24 +1587,24 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
           <t>electronics_components.xlsx</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="D12" t="inlineStr">
         <is>
           <t>Explore if there's a correlation between voltage and current.</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="E12" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F12" t="inlineStr">
         <is>
           <t>nan</t>
@@ -1455,6 +1656,11 @@
         </is>
       </c>
       <c r="P12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -1466,24 +1672,24 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
           <t>electronics_components.xlsx</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="D13" t="inlineStr">
         <is>
           <t>Create a scatter plot to visualize the relationship between frequency and inductance.</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="E13" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F13" t="inlineStr">
         <is>
           <t>nan</t>
@@ -1535,6 +1741,11 @@
         </is>
       </c>
       <c r="P13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q13" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -1546,24 +1757,24 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
           <t>electronics_components.xlsx</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="D14" t="inlineStr">
         <is>
           <t>Histogram of voltage values in the dataset.</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="E14" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F14" t="inlineStr">
         <is>
           <t>nan</t>
@@ -1615,6 +1826,11 @@
         </is>
       </c>
       <c r="P14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q14" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -1626,24 +1842,24 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
           <t>chemicals_1.xlsx</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="D15" t="inlineStr">
         <is>
           <t>Find the top 10 experiments with the highest yield.</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="E15" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F15" t="inlineStr">
         <is>
           <t>nan</t>
@@ -1695,6 +1911,11 @@
         </is>
       </c>
       <c r="P15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q15" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -1706,24 +1927,24 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
           <t>chemicals_1.xlsx</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="D16" t="inlineStr">
         <is>
           <t>Calculate the average concentration of chemicals used across all experiments.</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="E16" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F16" t="inlineStr">
         <is>
           <t>nan</t>
@@ -1775,6 +1996,11 @@
         </is>
       </c>
       <c r="P16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q16" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -1786,24 +2012,24 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
           <t>chemicals_1.xlsx</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="D17" t="inlineStr">
         <is>
           <t>Identify the experiment where the color change had the highest red (R) values.</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
+      <c r="E17" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F17" t="inlineStr">
         <is>
           <t>nan</t>
@@ -1855,6 +2081,11 @@
         </is>
       </c>
       <c r="P17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q17" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -1866,24 +2097,24 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
           <t>chemicals_1.xlsx</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="D18" t="inlineStr">
         <is>
           <t>Is there a correlation between higher temperatures and shorter reaction times?</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
+      <c r="E18" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F18" t="inlineStr">
         <is>
           <t>nan</t>
@@ -1935,6 +2166,11 @@
         </is>
       </c>
       <c r="P18" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q18" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -1946,24 +2182,24 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
           <t>chemicals_1.xlsx</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="D19" t="inlineStr">
         <is>
           <t>Find the experiment with the largest volume and the chemical used in it.</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
+      <c r="E19" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F19" t="inlineStr">
         <is>
           <t>nan</t>
@@ -2015,6 +2251,11 @@
         </is>
       </c>
       <c r="P19" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q19" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -2026,24 +2267,24 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
           <t>chemicals_1.xlsx</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="D20" t="inlineStr">
         <is>
           <t>Determine the pH level most commonly observed across all experiments.</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
+      <c r="E20" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F20" t="inlineStr">
         <is>
           <t>nan</t>
@@ -2095,6 +2336,11 @@
         </is>
       </c>
       <c r="P20" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q20" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -2106,24 +2352,24 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
           <t>chemicals_1.xlsx</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="D21" t="inlineStr">
         <is>
           <t>covariance between concentration and yield?</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
+      <c r="E21" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F21" t="inlineStr">
         <is>
           <t>nan</t>
@@ -2175,6 +2421,11 @@
         </is>
       </c>
       <c r="P21" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q21" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -2186,24 +2437,24 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
           <t>chemicals_1.xlsx</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
+      <c r="D22" t="inlineStr">
         <is>
           <t>Scatter plot to visualize the relationship between temperature and reaction time.</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
+      <c r="E22" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F22" t="inlineStr">
         <is>
           <t>nan</t>
@@ -2255,6 +2506,11 @@
         </is>
       </c>
       <c r="P22" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q22" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -2266,24 +2522,24 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
           <t>chemicals_1.xlsx</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
+      <c r="D23" t="inlineStr">
         <is>
           <t>Analyze the correlation between volume and concentration levels in the experiments.</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
+      <c r="E23" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F23" t="inlineStr">
         <is>
           <t>nan</t>
@@ -2335,6 +2591,11 @@
         </is>
       </c>
       <c r="P23" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q23" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -2346,24 +2607,24 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
           <t>SolarPanels.xlsx</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
+      <c r="D24" t="inlineStr">
         <is>
           <t>What are 3 panel ids with largest power output?</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
+      <c r="E24" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F24" t="inlineStr">
         <is>
           <t>nan</t>
@@ -2415,6 +2676,11 @@
         </is>
       </c>
       <c r="P24" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q24" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -2426,24 +2692,24 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
           <t>SolarPanels.xlsx</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
+      <c r="D25" t="inlineStr">
         <is>
           <t>Bar plot of 11 smallest temperatures</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
+      <c r="E25" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F25" t="inlineStr">
         <is>
           <t>nan</t>
@@ -2495,6 +2761,11 @@
         </is>
       </c>
       <c r="P25" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q25" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -2506,24 +2777,24 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
           <t>SolarPanels.xlsx</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
+      <c r="D26" t="inlineStr">
         <is>
           <t>Find average light intensity. Subtract 40 from it and multiply by 2 afterwards.</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr">
+      <c r="E26" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F26" t="inlineStr">
         <is>
           <t>nan</t>
@@ -2575,6 +2846,11 @@
         </is>
       </c>
       <c r="P26" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q26" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -2586,24 +2862,24 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
           <t>SolarPanels.xlsx</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
+      <c r="D27" t="inlineStr">
         <is>
           <t>Find 3 rows with the biggest voltage output. Create a grouped bar chart with voltage and current outputs from the found rows.</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr">
+      <c r="E27" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F27" t="inlineStr">
         <is>
           <t>nan</t>
@@ -2655,6 +2931,11 @@
         </is>
       </c>
       <c r="P27" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q27" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -2666,24 +2947,24 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
           <t>SolarPanels.xlsx</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
+      <c r="D28" t="inlineStr">
         <is>
           <t>How much more often does High efficiency occur than Low?</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr">
+      <c r="E28" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F28" t="inlineStr">
         <is>
           <t>nan</t>
@@ -2735,6 +3016,11 @@
         </is>
       </c>
       <c r="P28" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q28" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -2746,24 +3032,24 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
           <t>medical_trial.xlsx</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
+      <c r="D29" t="inlineStr">
         <is>
           <t>correlation between blood pressure and heart rate</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr">
+      <c r="E29" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F29" t="inlineStr">
         <is>
           <t>nan</t>
@@ -2815,6 +3101,11 @@
         </is>
       </c>
       <c r="P29" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q29" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -2826,24 +3117,24 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
+          <t>28</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
           <t>medical_trial.xlsx</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr">
+      <c r="D30" t="inlineStr">
         <is>
           <t>is there any patient with nausea side effect? If there is, give me the patient's id</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr">
+      <c r="E30" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F30" t="inlineStr">
         <is>
           <t>nan</t>
@@ -2895,6 +3186,11 @@
         </is>
       </c>
       <c r="P30" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q30" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -2906,24 +3202,24 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
           <t>medical_trial.xlsx</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr">
+      <c r="D31" t="inlineStr">
         <is>
           <t>Draw a bar plot with the 3 shortest recovery times. Use red color.</t>
         </is>
       </c>
-      <c r="D31" t="inlineStr">
+      <c r="E31" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F31" t="inlineStr">
         <is>
           <t>nan</t>
@@ -2975,6 +3271,11 @@
         </is>
       </c>
       <c r="P31" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q31" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -2986,24 +3287,24 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
           <t>medical_trial.xlsx</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr">
+      <c r="D32" t="inlineStr">
         <is>
           <t>What is the most frequent side effect?</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr">
+      <c r="E32" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F32" t="inlineStr">
         <is>
           <t>nan</t>
@@ -3055,6 +3356,11 @@
         </is>
       </c>
       <c r="P32" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q32" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -3066,24 +3372,24 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
+          <t>31</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
           <t>agriculture_analysis.xlsx</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr">
+      <c r="D33" t="inlineStr">
         <is>
           <t>Find the pH Level of Rice</t>
         </is>
       </c>
-      <c r="D33" t="inlineStr">
+      <c r="E33" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F33" t="inlineStr">
         <is>
           <t>nan</t>
@@ -3135,6 +3441,11 @@
         </is>
       </c>
       <c r="P33" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q33" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -3146,24 +3457,24 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
           <t>agriculture_analysis.xlsx</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr">
+      <c r="D34" t="inlineStr">
         <is>
           <t>What is the average moisture for the crops with pH level of 7?</t>
         </is>
       </c>
-      <c r="D34" t="inlineStr">
+      <c r="E34" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F34" t="inlineStr">
         <is>
           <t>nan</t>
@@ -3215,6 +3526,11 @@
         </is>
       </c>
       <c r="P34" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q34" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -3226,24 +3542,24 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
           <t>agriculture_analysis.xlsx</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr">
+      <c r="D35" t="inlineStr">
         <is>
           <t>Line plot the temperature column, but each value divided by 2</t>
         </is>
       </c>
-      <c r="D35" t="inlineStr">
+      <c r="E35" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F35" t="inlineStr">
         <is>
           <t>nan</t>
@@ -3295,6 +3611,11 @@
         </is>
       </c>
       <c r="P35" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q35" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -3306,24 +3627,24 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
           <t>agriculture_analysis.xlsx</t>
         </is>
       </c>
-      <c r="C36" t="inlineStr">
+      <c r="D36" t="inlineStr">
         <is>
           <t>What is the 3rd largest yield value?</t>
         </is>
       </c>
-      <c r="D36" t="inlineStr">
+      <c r="E36" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F36" t="inlineStr">
         <is>
           <t>nan</t>
@@ -3375,6 +3696,11 @@
         </is>
       </c>
       <c r="P36" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q36" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -3386,24 +3712,24 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
           <t>geological.xlsx</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr">
+      <c r="D37" t="inlineStr">
         <is>
           <t>What is the correlation between porosity and susceptibility</t>
         </is>
       </c>
-      <c r="D37" t="inlineStr">
+      <c r="E37" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F37" t="inlineStr">
         <is>
           <t>nan</t>
@@ -3455,6 +3781,11 @@
         </is>
       </c>
       <c r="P37" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q37" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -3466,24 +3797,24 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
+          <t>36</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
           <t>geological.xlsx</t>
         </is>
       </c>
-      <c r="C38" t="inlineStr">
+      <c r="D38" t="inlineStr">
         <is>
           <t>the biggest depth</t>
         </is>
       </c>
-      <c r="D38" t="inlineStr">
+      <c r="E38" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F38" t="inlineStr">
         <is>
           <t>nan</t>
@@ -3535,6 +3866,11 @@
         </is>
       </c>
       <c r="P38" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q38" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -3546,24 +3882,24 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
+          <t>37</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
           <t>geological.xlsx</t>
         </is>
       </c>
-      <c r="C39" t="inlineStr">
+      <c r="D39" t="inlineStr">
         <is>
           <t>boxplot of seismic velocity and density columns</t>
         </is>
       </c>
-      <c r="D39" t="inlineStr">
+      <c r="E39" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F39" t="inlineStr">
         <is>
           <t>nan</t>
@@ -3615,6 +3951,11 @@
         </is>
       </c>
       <c r="P39" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q39" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -3626,24 +3967,24 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
+          <t>38</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
           <t>geological.xlsx</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr">
+      <c r="D40" t="inlineStr">
         <is>
           <t>pie plot the 3 smallest permeabilities. Add rock types to the legend.</t>
         </is>
       </c>
-      <c r="D40" t="inlineStr">
+      <c r="E40" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F40" t="inlineStr">
         <is>
           <t>nan</t>
@@ -3695,6 +4036,11 @@
         </is>
       </c>
       <c r="P40" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q40" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -3706,24 +4052,24 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
           <t>energy_consumption.xlsx</t>
         </is>
       </c>
-      <c r="C41" t="inlineStr">
+      <c r="D41" t="inlineStr">
         <is>
           <t>What are three device ids with the largest use duration</t>
         </is>
       </c>
-      <c r="D41" t="inlineStr">
+      <c r="E41" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F41" t="inlineStr">
         <is>
           <t>nan</t>
@@ -3775,6 +4121,11 @@
         </is>
       </c>
       <c r="P41" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q41" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -3786,24 +4137,24 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
           <t>energy_consumption.xlsx</t>
         </is>
       </c>
-      <c r="C42" t="inlineStr">
+      <c r="D42" t="inlineStr">
         <is>
           <t>Find the correlation between energy cost and power consumption</t>
         </is>
       </c>
-      <c r="D42" t="inlineStr">
+      <c r="E42" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F42" t="inlineStr">
         <is>
           <t>nan</t>
@@ -3855,6 +4206,11 @@
         </is>
       </c>
       <c r="P42" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q42" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -3866,24 +4222,24 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
+          <t>41</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
           <t>energy_consumption.xlsx</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr">
+      <c r="D43" t="inlineStr">
         <is>
           <t>Pie plot 6 usage durations with largest values. State the device ids in the legend</t>
         </is>
       </c>
-      <c r="D43" t="inlineStr">
+      <c r="E43" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F43" t="inlineStr">
         <is>
           <t>nan</t>
@@ -3935,6 +4291,11 @@
         </is>
       </c>
       <c r="P43" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q43" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -3946,24 +4307,24 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
+          <t>42</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
           <t>energy_consumption.xlsx</t>
         </is>
       </c>
-      <c r="C44" t="inlineStr">
+      <c r="D44" t="inlineStr">
         <is>
           <t>Is there any voltage fluctuation bigger than 3000? Reply yes or no</t>
         </is>
       </c>
-      <c r="D44" t="inlineStr">
+      <c r="E44" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F44" t="inlineStr">
         <is>
           <t>nan</t>
@@ -4015,6 +4376,11 @@
         </is>
       </c>
       <c r="P44" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q44" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -4026,24 +4392,24 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
+          <t>43</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
           <t>genetics_sic.xlsx</t>
         </is>
       </c>
-      <c r="C45" t="inlineStr">
+      <c r="D45" t="inlineStr">
         <is>
           <t>Find the most common base pair</t>
         </is>
       </c>
-      <c r="D45" t="inlineStr">
+      <c r="E45" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F45" t="inlineStr">
         <is>
           <t>nan</t>
@@ -4095,6 +4461,11 @@
         </is>
       </c>
       <c r="P45" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q45" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -4106,24 +4477,24 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
+          <t>44</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
           <t>genetics_sic.xlsx</t>
         </is>
       </c>
-      <c r="C46" t="inlineStr">
+      <c r="D46" t="inlineStr">
         <is>
           <t>What is the average mutation rate for the rows with protein synthesis rate higher than 228.</t>
         </is>
       </c>
-      <c r="D46" t="inlineStr">
+      <c r="E46" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F46" t="inlineStr">
         <is>
           <t>nan</t>
@@ -4175,6 +4546,11 @@
         </is>
       </c>
       <c r="P46" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q46" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -4186,24 +4562,24 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
           <t>genetics_sic.xlsx</t>
         </is>
       </c>
-      <c r="C47" t="inlineStr">
+      <c r="D47" t="inlineStr">
         <is>
           <t>Determine the id of a sequence that has the highest gene expression</t>
         </is>
       </c>
-      <c r="D47" t="inlineStr">
+      <c r="E47" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F47" t="inlineStr">
         <is>
           <t>nan</t>
@@ -4255,6 +4631,11 @@
         </is>
       </c>
       <c r="P47" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q47" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -4266,24 +4647,24 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
+          <t>46</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
           <t>genetics_sic.xlsx</t>
         </is>
       </c>
-      <c r="C48" t="inlineStr">
+      <c r="D48" t="inlineStr">
         <is>
           <t>Plot of 4 smallest synthesis rates with title: Report 2021Q1. Place sequence ids on the x axis.</t>
         </is>
       </c>
-      <c r="D48" t="inlineStr">
+      <c r="E48" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F48" t="inlineStr">
         <is>
           <t>nan</t>
@@ -4335,6 +4716,11 @@
         </is>
       </c>
       <c r="P48" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q48" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -4346,24 +4732,24 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
+          <t>47</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
           <t>robotics_sensors.xlsx</t>
         </is>
       </c>
-      <c r="C49" t="inlineStr">
+      <c r="D49" t="inlineStr">
         <is>
           <t>How big is the correlation between temperature and voltage?</t>
         </is>
       </c>
-      <c r="D49" t="inlineStr">
+      <c r="E49" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F49" t="inlineStr">
         <is>
           <t>nan</t>
@@ -4415,6 +4801,11 @@
         </is>
       </c>
       <c r="P49" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q49" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -4426,24 +4817,24 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
+          <t>48</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
           <t>robotics_sensors.xlsx</t>
         </is>
       </c>
-      <c r="C50" t="inlineStr">
+      <c r="D50" t="inlineStr">
         <is>
           <t>Find the most frequent error code</t>
         </is>
       </c>
-      <c r="D50" t="inlineStr">
+      <c r="E50" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F50" t="inlineStr">
         <is>
           <t>nan</t>
@@ -4495,6 +4886,11 @@
         </is>
       </c>
       <c r="P50" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q50" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -4506,24 +4902,24 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
+          <t>49</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
           <t>robotics_sensors.xlsx</t>
         </is>
       </c>
-      <c r="C51" t="inlineStr">
+      <c r="D51" t="inlineStr">
         <is>
           <t>Barplot 9 biggest object detection counts. Place robot id on x-axis and set title to Top 9 counts</t>
         </is>
       </c>
-      <c r="D51" t="inlineStr">
+      <c r="E51" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F51" t="inlineStr">
         <is>
           <t>nan</t>
@@ -4575,6 +4971,11 @@
         </is>
       </c>
       <c r="P51" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q51" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -4586,24 +4987,24 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
           <t>robotics_sensors.xlsx</t>
         </is>
       </c>
-      <c r="C52" t="inlineStr">
+      <c r="D52" t="inlineStr">
         <is>
           <t>Create a scatter plot with voltage on x axis and temperature on y axis</t>
         </is>
       </c>
-      <c r="D52" t="inlineStr">
+      <c r="E52" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F52" t="inlineStr">
         <is>
           <t>nan</t>
@@ -4655,6 +5056,11 @@
         </is>
       </c>
       <c r="P52" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q52" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -4666,24 +5072,24 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
           <t>financial_market_data.xlsx</t>
         </is>
       </c>
-      <c r="C53" t="inlineStr">
+      <c r="D53" t="inlineStr">
         <is>
           <t>Bar plot of the 7 biggest eps</t>
         </is>
       </c>
-      <c r="D53" t="inlineStr">
+      <c r="E53" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F53" t="inlineStr">
         <is>
           <t>nan</t>
@@ -4735,6 +5141,11 @@
         </is>
       </c>
       <c r="P53" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q53" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -4746,24 +5157,24 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
           <t>financial_market_data.xlsx</t>
         </is>
       </c>
-      <c r="C54" t="inlineStr">
+      <c r="D54" t="inlineStr">
         <is>
           <t>What is the second lowest price</t>
         </is>
       </c>
-      <c r="D54" t="inlineStr">
+      <c r="E54" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F54" t="inlineStr">
         <is>
           <t>nan</t>
@@ -4815,6 +5226,11 @@
         </is>
       </c>
       <c r="P54" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q54" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -4826,24 +5242,24 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
           <t>financial_market_data.xlsx</t>
         </is>
       </c>
-      <c r="C55" t="inlineStr">
+      <c r="D55" t="inlineStr">
         <is>
           <t>Can you please generate me a pie plot of 4 smallest volumes with the prices depicted on the legend? Thank you.</t>
         </is>
       </c>
-      <c r="D55" t="inlineStr">
+      <c r="E55" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F55" t="inlineStr">
         <is>
           <t>nan</t>
@@ -4895,6 +5311,11 @@
         </is>
       </c>
       <c r="P55" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q55" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -4906,24 +5327,24 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
           <t>financial_market_data.xlsx</t>
         </is>
       </c>
-      <c r="C56" t="inlineStr">
+      <c r="D56" t="inlineStr">
         <is>
           <t>Add the PE ratio column to the EPS column and find the minimal value of this sum.</t>
         </is>
       </c>
-      <c r="D56" t="inlineStr">
+      <c r="E56" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F56" t="inlineStr">
         <is>
           <t>nan</t>
@@ -4975,6 +5396,11 @@
         </is>
       </c>
       <c r="P56" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q56" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -4986,24 +5412,24 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
           <t>biomedical_image_analysis.xlsx</t>
         </is>
       </c>
-      <c r="C57" t="inlineStr">
+      <c r="D57" t="inlineStr">
         <is>
           <t>Find the correlation between SNR and tissue density</t>
         </is>
       </c>
-      <c r="D57" t="inlineStr">
+      <c r="E57" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F57" t="inlineStr">
         <is>
           <t>nan</t>
@@ -5055,6 +5481,11 @@
         </is>
       </c>
       <c r="P57" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q57" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -5066,24 +5497,24 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
+          <t>56</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
           <t>biomedical_image_analysis.xlsx</t>
         </is>
       </c>
-      <c r="C58" t="inlineStr">
+      <c r="D58" t="inlineStr">
         <is>
           <t>Find the average image processing time between the images with pixel intensity less than 200.</t>
         </is>
       </c>
-      <c r="D58" t="inlineStr">
+      <c r="E58" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="E58" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F58" t="inlineStr">
         <is>
           <t>nan</t>
@@ -5135,6 +5566,11 @@
         </is>
       </c>
       <c r="P58" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q58" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -5146,24 +5582,24 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
+          <t>57</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
           <t>biomedical_image_analysis.xlsx</t>
         </is>
       </c>
-      <c r="C59" t="inlineStr">
+      <c r="D59" t="inlineStr">
         <is>
           <t>Plot the first 10 tissue density values that occur in the table and add their id on x-axis.</t>
         </is>
       </c>
-      <c r="D59" t="inlineStr">
+      <c r="E59" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="E59" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F59" t="inlineStr">
         <is>
           <t>nan</t>
@@ -5215,6 +5651,11 @@
         </is>
       </c>
       <c r="P59" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q59" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -5226,24 +5667,24 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
+          <t>58</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
           <t>biomedical_image_analysis.xlsx</t>
         </is>
       </c>
-      <c r="C60" t="inlineStr">
+      <c r="D60" t="inlineStr">
         <is>
           <t>Is the average contrast value bigger than the average pixel intensity?</t>
         </is>
       </c>
-      <c r="D60" t="inlineStr">
+      <c r="E60" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="E60" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F60" t="inlineStr">
         <is>
           <t>nan</t>
@@ -5295,6 +5736,11 @@
         </is>
       </c>
       <c r="P60" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q60" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -5306,24 +5752,24 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
+          <t>59</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
           <t>biomedical_image_analysis.xlsx</t>
         </is>
       </c>
-      <c r="C61" t="inlineStr">
+      <c r="D61" t="inlineStr">
         <is>
           <t>How big is the image processing time for image with id of 27</t>
         </is>
       </c>
-      <c r="D61" t="inlineStr">
+      <c r="E61" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="E61" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F61" t="inlineStr">
         <is>
           <t>nan</t>
@@ -5375,6 +5821,11 @@
         </is>
       </c>
       <c r="P61" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q61" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -5386,24 +5837,24 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
           <t>porsche_tmp.xlsx</t>
         </is>
       </c>
-      <c r="C62" t="inlineStr">
+      <c r="D62" t="inlineStr">
         <is>
           <t>Identify the model variant with the highest price, along with it’s color</t>
         </is>
       </c>
-      <c r="D62" t="inlineStr">
+      <c r="E62" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="E62" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F62" t="inlineStr">
         <is>
           <t>nan</t>
@@ -5455,6 +5906,11 @@
         </is>
       </c>
       <c r="P62" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q62" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -5466,24 +5922,24 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
+          <t>61</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
           <t>porsche_tmp.xlsx</t>
         </is>
       </c>
-      <c r="C63" t="inlineStr">
+      <c r="D63" t="inlineStr">
         <is>
           <t>Determine which model variant has the best acceleration.</t>
         </is>
       </c>
-      <c r="D63" t="inlineStr">
+      <c r="E63" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="E63" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F63" t="inlineStr">
         <is>
           <t>nan</t>
@@ -5535,6 +5991,11 @@
         </is>
       </c>
       <c r="P63" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q63" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -5546,24 +6007,24 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
+          <t>62</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
           <t>porsche_tmp.xlsx</t>
         </is>
       </c>
-      <c r="C64" t="inlineStr">
+      <c r="D64" t="inlineStr">
         <is>
           <t>Bar plot the torque for each model. Use green color for the plot.</t>
         </is>
       </c>
-      <c r="D64" t="inlineStr">
+      <c r="E64" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="E64" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F64" t="inlineStr">
         <is>
           <t>nan</t>
@@ -5615,6 +6076,11 @@
         </is>
       </c>
       <c r="P64" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q64" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -5626,24 +6092,24 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
+          <t>63</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
           <t>porsche_tmp.xlsx</t>
         </is>
       </c>
-      <c r="C65" t="inlineStr">
+      <c r="D65" t="inlineStr">
         <is>
           <t>Plot the frequency of wheel types. Place wheel type on x-axis and the amount of times it occurs on y-axis.</t>
         </is>
       </c>
-      <c r="D65" t="inlineStr">
+      <c r="E65" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="E65" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F65" t="inlineStr">
         <is>
           <t>nan</t>
@@ -5695,6 +6161,11 @@
         </is>
       </c>
       <c r="P65" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q65" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -5706,24 +6177,24 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
+          <t>64</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
           <t>porsche_tmp.xlsx</t>
         </is>
       </c>
-      <c r="C66" t="inlineStr">
+      <c r="D66" t="inlineStr">
         <is>
           <t>correlation between price and acceleration</t>
         </is>
       </c>
-      <c r="D66" t="inlineStr">
+      <c r="E66" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="E66" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F66" t="inlineStr">
         <is>
           <t>nan</t>
@@ -5775,6 +6246,11 @@
         </is>
       </c>
       <c r="P66" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q66" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -5786,24 +6262,24 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
           <t>porsche_tmp.xlsx</t>
         </is>
       </c>
-      <c r="C67" t="inlineStr">
+      <c r="D67" t="inlineStr">
         <is>
           <t>What is the price of the smallest battery capacity model?</t>
         </is>
       </c>
-      <c r="D67" t="inlineStr">
+      <c r="E67" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="E67" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F67" t="inlineStr">
         <is>
           <t>nan</t>
@@ -5855,6 +6331,11 @@
         </is>
       </c>
       <c r="P67" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q67" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -5866,24 +6347,24 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
+          <t>66</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
           <t>porsche_tmp.xlsx</t>
         </is>
       </c>
-      <c r="C68" t="inlineStr">
+      <c r="D68" t="inlineStr">
         <is>
           <t>What are all available wheel types?</t>
         </is>
       </c>
-      <c r="D68" t="inlineStr">
+      <c r="E68" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="E68" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F68" t="inlineStr">
         <is>
           <t>nan</t>
@@ -5935,6 +6416,11 @@
         </is>
       </c>
       <c r="P68" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q68" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -5946,24 +6432,24 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
+          <t>67</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
           <t>skoda_warehouse.xlsx</t>
         </is>
       </c>
-      <c r="C69" t="inlineStr">
+      <c r="D69" t="inlineStr">
         <is>
           <t>Identify the part with the highest total value (Total Value = Quantity in Stock * Unit Price).</t>
         </is>
       </c>
-      <c r="D69" t="inlineStr">
+      <c r="E69" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="E69" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F69" t="inlineStr">
         <is>
           <t>nan</t>
@@ -6015,6 +6501,11 @@
         </is>
       </c>
       <c r="P69" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q69" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -6026,24 +6517,24 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
+          <t>68</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
           <t>skoda_warehouse.xlsx</t>
         </is>
       </c>
-      <c r="C70" t="inlineStr">
+      <c r="D70" t="inlineStr">
         <is>
           <t>Calculate the average quantity in stock for all parts</t>
         </is>
       </c>
-      <c r="D70" t="inlineStr">
+      <c r="E70" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="E70" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F70" t="inlineStr">
         <is>
           <t>nan</t>
@@ -6095,6 +6586,11 @@
         </is>
       </c>
       <c r="P70" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q70" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -6106,24 +6602,24 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
+          <t>69</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
           <t>skoda_warehouse.xlsx</t>
         </is>
       </c>
-      <c r="C71" t="inlineStr">
+      <c r="D71" t="inlineStr">
         <is>
           <t>plot the highest unit price and the lowest unit price side by side</t>
         </is>
       </c>
-      <c r="D71" t="inlineStr">
+      <c r="E71" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="E71" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F71" t="inlineStr">
         <is>
           <t>nan</t>
@@ -6175,6 +6671,11 @@
         </is>
       </c>
       <c r="P71" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q71" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -6186,24 +6687,24 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
+          <t>70</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
           <t>skoda_warehouse.xlsx</t>
         </is>
       </c>
-      <c r="C72" t="inlineStr">
+      <c r="D72" t="inlineStr">
         <is>
           <t>What are restock dates from january to april (included)?</t>
         </is>
       </c>
-      <c r="D72" t="inlineStr">
+      <c r="E72" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="E72" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F72" t="inlineStr">
         <is>
           <t>nan</t>
@@ -6255,6 +6756,11 @@
         </is>
       </c>
       <c r="P72" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q72" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -6266,24 +6772,24 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
+          <t>71</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
           <t>skoda_warehouse.xlsx</t>
         </is>
       </c>
-      <c r="C73" t="inlineStr">
+      <c r="D73" t="inlineStr">
         <is>
           <t>Determine the part number with smallest unit price that has it‘s quantity &gt; 600</t>
         </is>
       </c>
-      <c r="D73" t="inlineStr">
+      <c r="E73" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="E73" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F73" t="inlineStr">
         <is>
           <t>nan</t>
@@ -6335,6 +6841,11 @@
         </is>
       </c>
       <c r="P73" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q73" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -6346,24 +6857,24 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
+          <t>72</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
           <t>skoda_warehouse.xlsx</t>
         </is>
       </c>
-      <c r="C74" t="inlineStr">
+      <c r="D74" t="inlineStr">
         <is>
           <t>Create a histogram with quantity in stock on y-axis of 7 parts with the biggest unit prices</t>
         </is>
       </c>
-      <c r="D74" t="inlineStr">
+      <c r="E74" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="E74" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F74" t="inlineStr">
         <is>
           <t>nan</t>
@@ -6415,6 +6926,11 @@
         </is>
       </c>
       <c r="P74" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q74" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -6426,24 +6942,24 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
+          <t>73</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
           <t>skoda_warehouse.xlsx</t>
         </is>
       </c>
-      <c r="C75" t="inlineStr">
+      <c r="D75" t="inlineStr">
         <is>
           <t>What are the last two restock dates?</t>
         </is>
       </c>
-      <c r="D75" t="inlineStr">
+      <c r="E75" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="E75" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F75" t="inlineStr">
         <is>
           <t>nan</t>
@@ -6495,6 +7011,11 @@
         </is>
       </c>
       <c r="P75" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q75" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -6506,24 +7027,24 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
+          <t>74</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
           <t>faculties_tech_uni.xlsx</t>
         </is>
       </c>
-      <c r="C76" t="inlineStr">
+      <c r="D76" t="inlineStr">
         <is>
           <t>Find the average proportion of males to females across faculties</t>
         </is>
       </c>
-      <c r="D76" t="inlineStr">
+      <c r="E76" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="E76" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F76" t="inlineStr">
         <is>
           <t>nan</t>
@@ -6575,6 +7096,11 @@
         </is>
       </c>
       <c r="P76" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q76" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -6586,24 +7112,24 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
+          <t>75</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
           <t>faculties_tech_uni.xlsx</t>
         </is>
       </c>
-      <c r="C77" t="inlineStr">
+      <c r="D77" t="inlineStr">
         <is>
           <t>Average number of international students</t>
         </is>
       </c>
-      <c r="D77" t="inlineStr">
+      <c r="E77" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="E77" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F77" t="inlineStr">
         <is>
           <t>nan</t>
@@ -6655,6 +7181,11 @@
         </is>
       </c>
       <c r="P77" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q77" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -6666,24 +7197,24 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
+          <t>76</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
           <t>faculties_tech_uni.xlsx</t>
         </is>
       </c>
-      <c r="C78" t="inlineStr">
+      <c r="D78" t="inlineStr">
         <is>
           <t>Determine the correlation between undergrads and graduates</t>
         </is>
       </c>
-      <c r="D78" t="inlineStr">
+      <c r="E78" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="E78" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F78" t="inlineStr">
         <is>
           <t>nan</t>
@@ -6735,6 +7266,11 @@
         </is>
       </c>
       <c r="P78" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q78" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -6746,24 +7282,24 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
+          <t>77</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
           <t>faculties_tech_uni.xlsx</t>
         </is>
       </c>
-      <c r="C79" t="inlineStr">
+      <c r="D79" t="inlineStr">
         <is>
           <t>Filter out the faculties that have less than a 1400 number of students</t>
         </is>
       </c>
-      <c r="D79" t="inlineStr">
+      <c r="E79" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="E79" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F79" t="inlineStr">
         <is>
           <t>nan</t>
@@ -6815,6 +7351,11 @@
         </is>
       </c>
       <c r="P79" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q79" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -6826,24 +7367,24 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
+          <t>78</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
           <t>faculties_tech_uni.xlsx</t>
         </is>
       </c>
-      <c r="C80" t="inlineStr">
+      <c r="D80" t="inlineStr">
         <is>
           <t>Divide the number of male students by the total number of students. Create a bar plot of this ratio on y-axis and faculty names on x-axis</t>
         </is>
       </c>
-      <c r="D80" t="inlineStr">
+      <c r="E80" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="E80" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F80" t="inlineStr">
         <is>
           <t>nan</t>
@@ -6895,6 +7436,11 @@
         </is>
       </c>
       <c r="P80" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q80" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -6906,24 +7452,24 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
+          <t>79</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
           <t>faculties_tech_uni.xlsx</t>
         </is>
       </c>
-      <c r="C81" t="inlineStr">
+      <c r="D81" t="inlineStr">
         <is>
           <t>Plot the average number of male students compared to the average number of female students</t>
         </is>
       </c>
-      <c r="D81" t="inlineStr">
+      <c r="E81" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="E81" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F81" t="inlineStr">
         <is>
           <t>nan</t>
@@ -6975,6 +7521,11 @@
         </is>
       </c>
       <c r="P81" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q81" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -6986,24 +7537,24 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
           <t>faculties_tech_uni.xlsx</t>
         </is>
       </c>
-      <c r="C82" t="inlineStr">
+      <c r="D82" t="inlineStr">
         <is>
           <t>Pie plot the number of international students. Put faculty names to the legend.</t>
         </is>
       </c>
-      <c r="D82" t="inlineStr">
+      <c r="E82" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="E82" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F82" t="inlineStr">
         <is>
           <t>nan</t>
@@ -7055,6 +7606,11 @@
         </is>
       </c>
       <c r="P82" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q82" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
@@ -7066,7 +7622,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>81</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -7076,14 +7632,14 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
           <t>26</t>
         </is>
       </c>
-      <c r="E83" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F83" t="inlineStr">
         <is>
           <t>nan</t>
@@ -7135,6 +7691,11 @@
         </is>
       </c>
       <c r="P83" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q83" t="inlineStr">
         <is>
           <t>nan</t>
         </is>

</xml_diff>